<commit_message>
Fixed the difficulty(color) of "messages"
</commit_message>
<xml_diff>
--- a/TestCases/Distribution of Teamwork.xlsx
+++ b/TestCases/Distribution of Teamwork.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Decho\Desktop\TestPlan\TestCases\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -17,8 +22,8 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -166,8 +171,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,28 +555,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="83.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="12" customFormat="1">
+    <row r="1" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -585,7 +590,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -599,7 +604,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -613,7 +618,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
@@ -624,7 +629,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -635,7 +640,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -646,7 +651,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -657,11 +662,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -675,19 +680,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="85.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -695,7 +700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -703,7 +708,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -711,7 +716,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -719,7 +724,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -727,7 +732,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -735,7 +740,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -743,7 +748,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -751,7 +756,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -765,19 +770,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -785,7 +790,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -793,7 +798,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -801,7 +806,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -815,19 +820,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="141.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -835,7 +840,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -843,7 +848,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -851,7 +856,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -859,7 +864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -867,7 +872,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -875,7 +880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -883,7 +888,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -891,7 +896,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -906,19 +911,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="83.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -926,7 +931,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -934,7 +939,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -942,7 +947,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -950,7 +955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -958,7 +963,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>

</xml_diff>